<commit_message>
Excel sheet, and my updated version numbers that hopefully won't collide with yours
</commit_message>
<xml_diff>
--- a/Docs/Excel/English and Spanish Translations.xlsx
+++ b/Docs/Excel/English and Spanish Translations.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Bald Builders\SESA\_A\_UX\OnSiteX\Docs\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\OnSiteX\Docs\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="279">
   <si>
     <t>home_title</t>
   </si>
@@ -766,12 +766,132 @@
 &lt;p&gt;If you submit too many hours, an exception for that shift will be marked with a red flag.&lt;/p&gt;
 &lt;p&gt;It is &lt;b&gt;your&lt;/b&gt; responsibility to make sure you document all hours worked. The hours you see on this screen will be the hours you are paid unless the hours are flagged (red flag).&lt;/p&gt;</t>
   </si>
+  <si>
+    <t>spinner_deleting_report</t>
+  </si>
+  <si>
+    <t>Deleting report...</t>
+  </si>
+  <si>
+    <t>Eliminar informe...</t>
+  </si>
+  <si>
+    <t>error_deleting_report_message</t>
+  </si>
+  <si>
+    <t>Error deleting report. Please try again later.</t>
+  </si>
+  <si>
+    <t>Error al eliminar el informe. Por favor, inténtelo de nuevo más tarde.</t>
+  </si>
+  <si>
+    <t>error_server_connect_message</t>
+  </si>
+  <si>
+    <t>Could not connect to server. Please try again later.</t>
+  </si>
+  <si>
+    <t>No se pudo conectar al servidor. Por favor, inténtelo de nuevo más tarde.</t>
+  </si>
+  <si>
+    <t>error_fetching_reports_title</t>
+  </si>
+  <si>
+    <t>Connection Error</t>
+  </si>
+  <si>
+    <t>Error de Conexión</t>
+  </si>
+  <si>
+    <t>error_fetching_reports_message</t>
+  </si>
+  <si>
+    <t>Could not connect to server to retrieve reports. Please try again later.</t>
+  </si>
+  <si>
+    <t>No se pudo conectar al servidor para recuperar informes. Por favor, inténtelo de nuevo más tarde.</t>
+  </si>
+  <si>
+    <t>hours_header</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>payroll_period</t>
+  </si>
+  <si>
+    <t>Payroll Period</t>
+  </si>
+  <si>
+    <t>Período de Nómina</t>
+  </si>
+  <si>
+    <t>pay_period</t>
+  </si>
+  <si>
+    <t>Pay Period</t>
+  </si>
+  <si>
+    <t>Período de Pago</t>
+  </si>
+  <si>
+    <t>messages_title</t>
+  </si>
+  <si>
+    <t>Messages from Tino</t>
+  </si>
+  <si>
+    <t>Mensajes de Tino</t>
+  </si>
+  <si>
+    <t>message_date</t>
+  </si>
+  <si>
+    <t>message_from</t>
+  </si>
+  <si>
+    <t>Sender</t>
+  </si>
+  <si>
+    <t>Remitente</t>
+  </si>
+  <si>
+    <t>message_subject</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Tema</t>
+  </si>
+  <si>
+    <t>message_done</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>messages_no_messages</t>
+  </si>
+  <si>
+    <t>No messages available</t>
+  </si>
+  <si>
+    <t>No hay mensajes disponibles</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -801,12 +921,18 @@
       <name val="Roboto Condensed Light"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -821,7 +947,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -840,6 +966,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1121,19 +1251,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="81.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="123.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="115.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
@@ -1144,7 +1275,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1286,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1166,7 +1297,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1177,7 +1308,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1188,7 +1319,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1199,7 +1330,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1210,7 +1341,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="395.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="409.5">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1352,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1232,7 +1363,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1243,7 +1374,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1254,7 +1385,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1265,7 +1396,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1276,7 +1407,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1287,7 +1418,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1298,7 +1429,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1309,7 +1440,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1320,7 +1451,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1462,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1342,7 +1473,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1353,7 +1484,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1364,7 +1495,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1375,7 +1506,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
@@ -1386,7 +1517,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1397,7 +1528,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
@@ -1408,7 +1539,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
@@ -1419,7 +1550,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -1430,7 +1561,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -1441,7 +1572,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
@@ -1452,7 +1583,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
         <v>17</v>
       </c>
@@ -1463,7 +1594,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
@@ -1474,7 +1605,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
@@ -1485,7 +1616,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
@@ -1496,7 +1627,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
@@ -1507,7 +1638,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
@@ -1518,7 +1649,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
@@ -1529,7 +1660,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
@@ -1540,7 +1671,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
         <v>35</v>
       </c>
@@ -1551,7 +1682,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="38.25">
       <c r="A39" s="5" t="s">
         <v>36</v>
       </c>
@@ -1562,7 +1693,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
         <v>37</v>
       </c>
@@ -1573,7 +1704,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
         <v>38</v>
       </c>
@@ -1584,7 +1715,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
         <v>39</v>
       </c>
@@ -1595,7 +1726,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
         <v>40</v>
       </c>
@@ -1606,7 +1737,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
         <v>41</v>
       </c>
@@ -1617,7 +1748,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
         <v>42</v>
       </c>
@@ -1628,7 +1759,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
         <v>43</v>
       </c>
@@ -1639,7 +1770,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
         <v>44</v>
       </c>
@@ -1650,7 +1781,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
         <v>45</v>
       </c>
@@ -1661,7 +1792,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
         <v>46</v>
       </c>
@@ -1672,7 +1803,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
         <v>47</v>
       </c>
@@ -1683,7 +1814,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
         <v>48</v>
       </c>
@@ -1694,7 +1825,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
@@ -1705,7 +1836,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="5" t="s">
         <v>50</v>
       </c>
@@ -1716,7 +1847,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="5" t="s">
         <v>51</v>
       </c>
@@ -1727,7 +1858,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
         <v>52</v>
       </c>
@@ -1738,7 +1869,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -1749,7 +1880,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="5" t="s">
         <v>54</v>
       </c>
@@ -1760,7 +1891,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="5" t="s">
         <v>55</v>
       </c>
@@ -1771,7 +1902,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="63.75">
       <c r="A59" s="5" t="s">
         <v>56</v>
       </c>
@@ -1782,7 +1913,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="5" t="s">
         <v>57</v>
       </c>
@@ -1793,7 +1924,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="25.5">
       <c r="A61" s="5" t="s">
         <v>58</v>
       </c>
@@ -1804,7 +1935,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
         <v>59</v>
       </c>
@@ -1815,7 +1946,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
         <v>60</v>
       </c>
@@ -1826,7 +1957,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
         <v>61</v>
       </c>
@@ -1837,7 +1968,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
         <v>62</v>
       </c>
@@ -1848,7 +1979,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="5" t="s">
         <v>63</v>
       </c>
@@ -1859,7 +1990,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
         <v>64</v>
       </c>
@@ -1870,7 +2001,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
         <v>65</v>
       </c>
@@ -1881,7 +2012,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
         <v>66</v>
       </c>
@@ -1892,7 +2023,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
         <v>67</v>
       </c>
@@ -1903,7 +2034,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
         <v>68</v>
       </c>
@@ -1914,7 +2045,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="5" t="s">
         <v>69</v>
       </c>
@@ -1925,7 +2056,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
         <v>70</v>
       </c>
@@ -1936,7 +2067,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="5" t="s">
         <v>71</v>
       </c>
@@ -1947,7 +2078,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
         <v>72</v>
       </c>
@@ -1958,7 +2089,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="5" t="s">
         <v>73</v>
       </c>
@@ -1969,7 +2100,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>74</v>
       </c>
@@ -1980,7 +2111,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="5" t="s">
         <v>75</v>
       </c>
@@ -1991,7 +2122,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="5" t="s">
         <v>76</v>
       </c>
@@ -2002,7 +2133,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="5" t="s">
         <v>77</v>
       </c>
@@ -2013,7 +2144,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
         <v>78</v>
       </c>
@@ -2024,7 +2155,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
         <v>79</v>
       </c>
@@ -2035,7 +2166,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
         <v>80</v>
       </c>
@@ -2046,7 +2177,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="5" t="s">
         <v>81</v>
       </c>
@@ -2057,7 +2188,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="5" t="s">
         <v>82</v>
       </c>
@@ -2066,6 +2197,160 @@
       </c>
       <c r="C85" s="6" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated strings in exel
</commit_message>
<xml_diff>
--- a/Docs/Excel/English and Spanish Translations.xlsx
+++ b/Docs/Excel/English and Spanish Translations.xlsx
@@ -864,7 +864,7 @@
     <t>&lt;p&gt;Shifts are numbered 1 through 7: Wednesday = Shift 1, Tuesday = Shift 2 etc.&lt;/p&gt;\n\n&lt;p&gt;Every payroll period has 7 shifts. If you do not work a shift, that shift still exists and you will have \"0\" hours for that shift.&lt;/p&gt;\n\n&lt;p&gt;A green checkbox will be displayed at the end of the shifts above when the hours in the work reports you have submitted for that shift are equal to the number of hours you should have worked for that shift.&lt;/p&gt;\n\n&lt;p&gt;If submitted hours are not equal to shift hours, that is not necessarily bad.The most important number(s) are the number of hours you worked and the total hours for the pay period (Wednesday through Tuesday of shifts 1through 7).&lt;/p&gt;\n\n&lt;p&gt;The number of hours submitted is the total of all shift hour submitted: this number is what will be used to calculate the hours in your paycheck.&lt;/p&gt;\n\n&lt;p&gt;Payroll Hours are the hours calculated from your hours submitted. This is thenumber of hours you should be paid for in your paycheck. However, payroll hours displayed here are UNVERIFIED hours.&lt;/p&gt;\n\n&lt;p&gt;If you made a mistake and sent &lt;b&gt;too many hours&lt;/b&gt;, then do not expect to see all of those hours on your paycheck.&lt;/p&gt;\n\n&lt;p&gt;If you have submitted &lt;b&gt;too few hours&lt;/b&gt;, it is your responsibility to correct them by submitting the appropriate work reports. &lt;b&gt;You will not be paid for hours not submitted (hours not reported).&lt;/b&gt;&lt;/p&gt;\n\n&lt;p&gt;Too few hours do not trigger a flag.&lt;/p&gt;\n\n&lt;p&gt;If you submit too many hours, an exception for that shift will be marked with a red flag.&lt;/p&gt;\n\n&lt;p&gt;It is &lt;b&gt;your&lt;/b&gt; responsibility to make sure you document all hours worked. The hours you see on this screen will be the hours you are paid unless the hours are flagged (red flag).&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Los turnos se numeran de 1 a 7: Miércoles = Turno 1, Martes = Turno 2, etc.&lt;/p&gt;\n\n&lt;p&gt;Cada período de nómina tiene 7 turnos. Si usted no trabaja un turno, ese turno todavía existe y usted tendrá \"0\" horas para ese turno.&lt;/p&gt;\n\n&lt;p&gt;Una casilla de verificación verde se mostrará al final de los turnos cuando las horas en los reportes que ha enviado para ese turno son iguales al número de horas que debería haber trabajado para ese turno.&lt;/p&gt;\n\n&lt;p&gt;Si las horas presentadas no son iguales a las horas de turno, eso no es necesariamente malo. Los números más importantes son el número de horas que trabajó y el número total de horas para el período de pago (de miércoles a martes de turnos de 1 a 7).&lt;/p&gt;\n\n&lt;p&gt;El total horas declaradas en sus reportes se utilizará para calcular las horas en su cheque de pago.&lt;/p&gt;\n\n&lt;p&gt;Horas de pago son calculadas a partir de aver sido enviadas. El número de horas sometidas debería ser, las horas mas la compensacion en su cheque. Sin embargo,los horas de nómina que se muestran aquí NO SON CONFIRMADAS.&lt;/p&gt;\n\n&lt;p&gt;Si usted cometió un error y envió demasiadas horas, entonces no espere ver todas esas horas en su cheque de pago.&lt;/p&gt;\n\n&lt;p&gt;Si ha sometido &lt;b&gt;menos horas&lt;/b&gt;, es &lt;b&gt;su&lt;/b&gt; responsabilidad corregirlas enviando los reportes de trabajo apropiados. &lt;b&gt;No se le pagará por horas no sometidas (las horas no reportadas).&lt;/b&gt;&lt;/p&gt;\n\n&lt;p&gt;Menos horas no activan una bandera.&lt;/p&gt;\n\n&lt;p&gt;Demasiadas horas activarán un bandera roja de error.&lt;/p&gt;\n\n&lt;p&gt;Es &lt;b&gt;su&lt;/b&gt; responsabilidad asegurarse de documentar todas las horas trabajadas. Las horas que ve en esta pantalla serán las horas que le pagen, a menos las horas que estén marcadas como una excepción (con una bandera roja).&lt;/p&gt;</t>
+    <t>&lt;p&gt;Los turnos se numeran de 1 a 7: Miércoles = Turno 1, Martes = Turno 2, etc.&lt;/p&gt;\n\n&lt;p&gt;Cada período de nómina tiene 7 turnos. Si usted no trabaja un turno, ese turno todavía existe y usted tendrá \"0\" horas para ese turno.&lt;/p&gt;\n\n&lt;p&gt;Una casilla de verificación verde se mostrará al final de los turnos cuando las horas enviadas para ese turno son iguales al número de horas que debería haber trabajado para ese turno.&lt;/p&gt;\n\n&lt;p&gt;Si las horas presentadas no son iguales a las horas de turno, eso no es necesariamente malo. Los números más importantes son el número de horas trabajadas y el número total de horas para el período de pago (de miércoles a martes de turnos de 1 a 7).&lt;/p&gt;\n\n&lt;p&gt;El total horas declaradas en sus reportes se utilizará para calcular las horas en su cheque de pago.&lt;/p&gt;\n\n&lt;p&gt;Horas de pago son calculadas a partir de aver sido enviadas. El número de horas sometidas seran las horas que se pagaran en su cheque. Sin embargo,las horas de nómina que se muestran aquí NO SON CONFIRMADAS.&lt;/p&gt;\n\n&lt;p&gt;Si usted cometió un error y envió demasiadas horas, entonces no espere ver todas esas horas en su cheque de pago.&lt;/p&gt;\n\n&lt;p&gt;Si ha sometido &lt;b&gt;menos horas&lt;/b&gt;, es &lt;b&gt;su&lt;/b&gt; responsabilidad corregirlas enviando los reportes de trabajo apropiados. &lt;b&gt;No se le pagará por horas no sometidas (las horas no reportadas).&lt;/b&gt;&lt;/p&gt;\n\n&lt;p&gt;Menos horas no activan una bandera.&lt;/p&gt;\n\n&lt;p&gt;Demasiadas horas activarán un bandera roja de error.&lt;/p&gt;\n\n&lt;p&gt;Es &lt;b&gt;su&lt;/b&gt; responsabilidad asegurarse de documentar todas las horas trabajadas. Las horas que ve en esta pantalla serán las horas que le pagen, a menos las horas que estén marcadas como una excepción (con una bandera roja).&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1233,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,7 +2057,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>56</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>58</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>249</v>
       </c>

</xml_diff>